<commit_message>
updated sendemail from python
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ideavat\AutomatedQA\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6C7B28-CC8F-486C-90EF-881EAA842BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20069DA-9997-4748-AAE6-ED18D6676A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -299,57 +299,12 @@
     <t>output</t>
   </si>
   <si>
-    <t>log</t>
-  </si>
-  <si>
-    <t>pabot --pabotlib --processes 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Reports </t>
   </si>
   <si>
     <t>basichotGuard.xml</t>
   </si>
   <si>
-    <t>Reports/executionLog.txt 2&gt;&amp;1</t>
-  </si>
-  <si>
-    <t>|| echo $(date +%F_%H:%M:%S)- BasicHotAbsoluteGuard/staleStatePrevention  execution failed &gt;&gt; Reports/executionLog.txt 2&gt;&amp;1</t>
-  </si>
-  <si>
-    <t>t23</t>
-  </si>
-  <si>
-    <t>t25</t>
-  </si>
-  <si>
-    <t>t26</t>
-  </si>
-  <si>
-    <t>t27</t>
-  </si>
-  <si>
-    <t>t28</t>
-  </si>
-  <si>
-    <t>t29</t>
-  </si>
-  <si>
-    <t>t30</t>
-  </si>
-  <si>
-    <t>t31</t>
-  </si>
-  <si>
-    <t>t32</t>
-  </si>
-  <si>
-    <t>t33</t>
-  </si>
-  <si>
-    <t>t34</t>
-  </si>
-  <si>
     <t>Guard1</t>
   </si>
   <si>
@@ -368,77 +323,27 @@
     <t>environment</t>
   </si>
   <si>
-    <t xml:space="preserve"> --name "Guard2_RSP-test_$(date +%F_%H:%M:%S)"</t>
-  </si>
-  <si>
     <t>Guard1_RSP-test</t>
   </si>
   <si>
     <t>BasicHotAbsoluteGuard</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF080808"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">--reporttitle </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF067D17"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>"BasicHotAbsoluteGuard"</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  --outputdir Reports </t>
-  </si>
-  <si>
     <t>Reports/cleanReports</t>
   </si>
   <si>
     <t>cleanReports.xml</t>
   </si>
   <si>
-    <t xml:space="preserve"> --output basichotGuard.xml </t>
-  </si>
-  <si>
     <t>groupname</t>
   </si>
   <si>
     <t>config146</t>
   </si>
   <si>
-    <t xml:space="preserve">config37 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> --variable environment:config146 </t>
-  </si>
-  <si>
     <t>RSP-test</t>
   </si>
   <si>
-    <t xml:space="preserve">  -v groupname:RSP-test </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -T $gt_path/basicHotAbsoluteGuardTest.robot $tc_path/staleStatePrevention.robot &gt;&gt; Reports/executionLog.txt 2&gt;&amp;1 || echo $(date +%F_%H:%M:%S)- BasicHotAbsoluteGuard/staleStatePrevention  execution failed &gt;&gt; Reports/executionLog.txt 2&gt;&amp;1</t>
-  </si>
-  <si>
     <t>testname</t>
   </si>
   <si>
@@ -448,13 +353,88 @@
     <t>cleanReports.robot</t>
   </si>
   <si>
-    <t>failurelog</t>
-  </si>
-  <si>
-    <t>override</t>
-  </si>
-  <si>
-    <t>executionLog.txt 2&gt;&amp;1</t>
+    <t xml:space="preserve">config146 </t>
+  </si>
+  <si>
+    <t>Guard2</t>
+  </si>
+  <si>
+    <t>Guard2_Imputes-test</t>
+  </si>
+  <si>
+    <t>DeadSensorGuard</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>deadSensorGuard.xml</t>
+  </si>
+  <si>
+    <t>Imputes-test</t>
+  </si>
+  <si>
+    <t>pabot --pabotlib --processes 2 --removekeywords passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deadSensorGuardTest.robot/staleStatePrevention.robot </t>
+  </si>
+  <si>
+    <t>Guard3</t>
+  </si>
+  <si>
+    <t>Guard4</t>
+  </si>
+  <si>
+    <t>Guard3_General-test</t>
+  </si>
+  <si>
+    <t>Guard4_General-test</t>
+  </si>
+  <si>
+    <t>HotGuard</t>
+  </si>
+  <si>
+    <t>GuardOrderMIX</t>
+  </si>
+  <si>
+    <t>guardOrderMIX.xml</t>
+  </si>
+  <si>
+    <t>hotGuard.xml</t>
+  </si>
+  <si>
+    <t>General-test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hotGuardTest.robot/staleStatePrevention.robot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardOrderMIXTest.robot/staleStatePrevention.robot </t>
+  </si>
+  <si>
+    <t>combinereport</t>
+  </si>
+  <si>
+    <t>GuardTest</t>
+  </si>
+  <si>
+    <t>Test performed on environment 146</t>
+  </si>
+  <si>
+    <t>basichotGuard.xml/deadSensorGuard.xml/hotGuard.xml /guardOrderMIX.xml</t>
+  </si>
+  <si>
+    <t>moveReports</t>
+  </si>
+  <si>
+    <t>rebot  --removekeywords passed</t>
+  </si>
+  <si>
+    <t>moveReports.xml</t>
+  </si>
+  <si>
+    <t>moveReports.robot</t>
   </si>
 </sst>
 </file>
@@ -464,7 +444,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,18 +461,6 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF0073BF"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF080808"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF067D17"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -550,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -596,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -884,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -1498,32 +1463,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="13.453125" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>84</v>
@@ -1532,154 +1496,203 @@
         <v>85</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>86</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="66" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="66" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.5">
+      <c r="A3" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5">
+      <c r="A4" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="43.5">
+      <c r="A5" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.5">
+      <c r="A6" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="58">
+      <c r="A7" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="101.5">
-      <c r="A3" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="29">
+      <c r="A8" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="101.5">
-      <c r="A4" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="F8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>103</v>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tues and wed file added
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Ideavat\AutomatedQA\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DCAF8D-097A-43B5-8108-86166FA07B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567D6663-C521-480C-8645-33966914EA8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
-    <sheet name="thursdaydaysuite" sheetId="2" r:id="rId2"/>
-    <sheet name="sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="tuesdaysuite" sheetId="3" r:id="rId2"/>
+    <sheet name="thursdaydaysuite" sheetId="2" r:id="rId3"/>
+    <sheet name="wednesdaydaysuite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="140">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -435,6 +436,27 @@
   </si>
   <si>
     <t>Test performed on environment 118</t>
+  </si>
+  <si>
+    <t>Guard1_RSP-test</t>
+  </si>
+  <si>
+    <t>RSP-test</t>
+  </si>
+  <si>
+    <t>Test performed on environment 37</t>
+  </si>
+  <si>
+    <t>config37</t>
+  </si>
+  <si>
+    <t>Test performed across different environment and different group</t>
+  </si>
+  <si>
+    <t>config91</t>
+  </si>
+  <si>
+    <t>Guard1_Imputes-test</t>
   </si>
 </sst>
 </file>
@@ -518,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -530,8 +552,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -857,41 +877,41 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="2.90625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="2.90625" style="18" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="2.90625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="2.90625" style="18" customWidth="1"/>
     <col min="7" max="7" width="23.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="2.90625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" style="18" customWidth="1"/>
     <col min="10" max="10" width="23.1796875" customWidth="1"/>
-    <col min="11" max="11" width="35.08984375" style="10" customWidth="1"/>
+    <col min="11" max="11" width="35.08984375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -899,25 +919,25 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="9">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>1</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="12">
         <v>50</v>
       </c>
     </row>
@@ -925,25 +945,25 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>2</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="12">
         <v>100</v>
       </c>
     </row>
@@ -951,25 +971,25 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="12">
         <v>9</v>
       </c>
     </row>
@@ -977,25 +997,25 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>1</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5" s="12">
         <v>95</v>
       </c>
     </row>
@@ -1003,25 +1023,25 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>2</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J6" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="12">
         <v>9</v>
       </c>
     </row>
@@ -1029,25 +1049,25 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="9">
         <v>99</v>
       </c>
     </row>
@@ -1055,25 +1075,25 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>200</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>5</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="9">
         <v>66</v>
       </c>
     </row>
@@ -1081,25 +1101,25 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>90</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="9">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="11">
+      <c r="H9" s="9">
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="9">
         <v>80.599999999999994</v>
       </c>
     </row>
@@ -1107,25 +1127,25 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="9">
         <v>88</v>
       </c>
     </row>
@@ -1133,25 +1153,25 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="9">
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="9">
         <v>64.400000000000006</v>
       </c>
     </row>
@@ -1159,25 +1179,25 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="9" t="s">
         <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="9">
         <v>60</v>
       </c>
     </row>
@@ -1185,25 +1205,25 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="9">
         <v>1</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1211,25 +1231,25 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>61</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="9">
         <v>2</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1237,25 +1257,25 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="9">
         <v>80.599999999999994</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="9">
         <v>20</v>
       </c>
     </row>
@@ -1263,25 +1283,25 @@
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="5">
         <v>100</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="9">
         <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="9">
         <v>88</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="11" t="s">
+      <c r="K16" s="9" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1289,19 +1309,19 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="9">
         <v>64.400000000000006</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="9">
         <v>70</v>
       </c>
     </row>
@@ -1309,13 +1329,13 @@
       <c r="G18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="9">
         <v>60</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="9">
         <v>100</v>
       </c>
     </row>
@@ -1323,13 +1343,13 @@
       <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H19" s="9" t="s">
         <v>58</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="9">
         <v>90</v>
       </c>
     </row>
@@ -1337,13 +1357,13 @@
       <c r="G20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="9" t="s">
         <v>59</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K20" s="9">
         <v>80</v>
       </c>
     </row>
@@ -1351,13 +1371,13 @@
       <c r="G21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>60</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K21" s="9">
         <v>66</v>
       </c>
     </row>
@@ -1365,13 +1385,13 @@
       <c r="G22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="9" t="s">
         <v>61</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="9">
         <v>60</v>
       </c>
     </row>
@@ -1379,13 +1399,13 @@
       <c r="G23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="9">
         <v>9</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K23" s="9">
         <v>50</v>
       </c>
     </row>
@@ -1393,13 +1413,13 @@
       <c r="G24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="9">
         <v>99</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="9">
         <v>75</v>
       </c>
     </row>
@@ -1407,13 +1427,13 @@
       <c r="G25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="11">
+      <c r="H25" s="9">
         <v>99</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="9">
         <v>100</v>
       </c>
     </row>
@@ -1421,13 +1441,13 @@
       <c r="G26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="11">
+      <c r="H26" s="9">
         <v>66</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="9">
         <v>50</v>
       </c>
     </row>
@@ -1435,7 +1455,7 @@
       <c r="J27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="9">
         <v>80</v>
       </c>
     </row>
@@ -1443,33 +1463,33 @@
       <c r="J28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="9">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="J29" s="2"/>
-      <c r="K29" s="11"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11">
       <c r="J30" s="2"/>
-      <c r="K30" s="11"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:11">
       <c r="J31" s="2"/>
-      <c r="K31" s="11"/>
+      <c r="K31" s="9"/>
     </row>
     <row r="32" spans="1:11">
       <c r="J32" s="2"/>
-      <c r="K32" s="11"/>
+      <c r="K32" s="9"/>
     </row>
     <row r="33" spans="10:11">
       <c r="J33" s="2"/>
-      <c r="K33" s="11"/>
+      <c r="K33" s="9"/>
     </row>
     <row r="34" spans="10:11">
       <c r="J34" s="2"/>
-      <c r="K34" s="11"/>
+      <c r="K34" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1479,11 +1499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1503,33 +1523,33 @@
       <c r="A1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="66" customHeight="1">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1544,21 +1564,21 @@
         <v>96</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.5">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>94</v>
@@ -1570,6 +1590,246 @@
         <v>88</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5">
+      <c r="A4" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29">
+      <c r="A5" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29">
+      <c r="A6" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="58">
+      <c r="A7" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="66" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.5">
+      <c r="A3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>131</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1580,7 +1840,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.5">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1601,7 +1861,7 @@
       <c r="G4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="17" t="s">
         <v>106</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1609,7 +1869,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="29">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1638,7 +1898,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="29">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1667,7 +1927,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="58">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>119</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1685,14 +1945,12 @@
       <c r="F7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>131</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1721,127 +1979,241 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
-  <dimension ref="A1:E17"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" customWidth="1"/>
-    <col min="3" max="3" width="2.90625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="66" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.5">
+      <c r="A3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="43.5">
+      <c r="A4" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29">
+      <c r="A5" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29">
+      <c r="A6" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="58">
+      <c r="A7" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AUQA-64_DataValidation-updated as per review comments
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753ABF9B-AD33-4565-803C-DB55487F9DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ABDB2-335F-48AD-A38E-4226405AE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,12 @@
     <sheet name="tuesdaysuite" sheetId="3" r:id="rId2"/>
     <sheet name="thursdaysuite" sheetId="2" r:id="rId3"/>
     <sheet name="wednesdaysuite" sheetId="4" r:id="rId4"/>
-    <sheet name="lists" sheetId="6" r:id="rId5"/>
+    <sheet name="commandinputdata" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="config37">lists!#REF!</definedName>
-    <definedName name="env">lists!#REF!</definedName>
-    <definedName name="environmane">lists!#REF!</definedName>
+    <definedName name="config37">commandinputdata!#REF!</definedName>
+    <definedName name="env">commandinputdata!#REF!</definedName>
+    <definedName name="environmane">commandinputdata!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="142">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -530,7 +530,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -621,24 +621,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,7 +1551,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1604,22 +1601,22 @@
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="23"/>
-      <c r="I2" s="22" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="23" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1627,28 +1624,28 @@
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1656,28 +1653,28 @@
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="23" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1685,28 +1682,28 @@
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="23" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1714,28 +1711,28 @@
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1743,45 +1740,45 @@
       <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="22" t="s">
+      <c r="H8" s="24"/>
+      <c r="I8" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1791,18 +1788,24 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{14A7592A-28A5-4DA8-BBFA-A088B6DA0243}">
           <x14:formula1>
-            <xm:f>lists!$A$2:$A$6</xm:f>
+            <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>G8 G2:G6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{67438C2C-B12B-431F-81E3-DC6C78F3EFCA}">
           <x14:formula1>
-            <xm:f>lists!$B$2:$B$4</xm:f>
+            <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{194D7DBB-6A47-4A01-B0E1-8E05DB433025}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1814,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1836,7 +1839,7 @@
       <c r="A1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="22" t="s">
         <v>90</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -1862,187 +1865,187 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="66" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="22" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="23" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.5">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.5">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="23" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="29">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="23" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="58">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="22" t="s">
+      <c r="H8" s="24"/>
+      <c r="I8" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2053,18 +2056,24 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{DE91018C-5078-4E02-9DE9-776D1975C9B1}">
           <x14:formula1>
-            <xm:f>lists!$A$2:$A$6</xm:f>
+            <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>G8 G2:G6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{7B904523-E04A-4BBE-BEE8-FE5E9BFAB573}">
           <x14:formula1>
-            <xm:f>lists!$B$2:$B$4</xm:f>
+            <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{E2DA3C6A-EFA3-42EE-B40E-65186E01436B}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2077,7 +2086,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2098,7 +2107,7 @@
       <c r="A1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="22" t="s">
         <v>90</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -2124,187 +2133,187 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="66" customHeight="1">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="22" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="23" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="43.5">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="43.5">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="23" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="29">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="23" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="29">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="58">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="22"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="22" t="s">
+      <c r="H8" s="24"/>
+      <c r="I8" s="23" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2313,18 +2322,24 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{B0AA5AB9-597C-4DB1-A986-300FC9C6A1CB}">
           <x14:formula1>
-            <xm:f>lists!$B$2:$B$4</xm:f>
+            <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{5BD409E9-D297-4950-9F42-71743EE745AC}">
           <x14:formula1>
-            <xm:f>lists!$A$2:$A$6</xm:f>
+            <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G6 G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{0FE8A086-DD56-4244-814A-05D86BAEBBF3}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2334,62 +2349,91 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DEF5F6-4C46-448A-BFCD-A11C30C672D9}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B6" s="3"/>
+      <c r="C6" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="23" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AUQA-64_DataValidation-updated as per review comments1
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ABDB2-335F-48AD-A38E-4226405AE6D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C250763-E5DB-4AD4-90E2-40B0CCEB37D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="152">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -467,6 +467,36 @@
   </si>
   <si>
     <t>config146</t>
+  </si>
+  <si>
+    <t>guard1_name</t>
+  </si>
+  <si>
+    <t>Guard2_General-test</t>
+  </si>
+  <si>
+    <t>Guard2_RSP-test</t>
+  </si>
+  <si>
+    <t>Guard3_Imputes-test</t>
+  </si>
+  <si>
+    <t>Guard3_RSP-test</t>
+  </si>
+  <si>
+    <t>guard4_name</t>
+  </si>
+  <si>
+    <t>guard2_name</t>
+  </si>
+  <si>
+    <t>guard3_name</t>
+  </si>
+  <si>
+    <t>Guard4_Imputes-test</t>
+  </si>
+  <si>
+    <t>Guard4_RSP-test</t>
   </si>
 </sst>
 </file>
@@ -497,7 +527,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,13 +554,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -570,7 +594,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -605,13 +628,6 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -619,22 +635,16 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,41 +935,41 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="2.90625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.90625" style="14" customWidth="1"/>
     <col min="4" max="4" width="22.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="2.90625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.90625" style="14" customWidth="1"/>
     <col min="7" max="7" width="23.1796875" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="2.90625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" style="14" customWidth="1"/>
     <col min="10" max="10" width="23.1796875" customWidth="1"/>
-    <col min="11" max="11" width="35.08984375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="35.08984375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -967,25 +977,25 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="11">
         <v>50</v>
       </c>
     </row>
@@ -993,25 +1003,25 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>2</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>100</v>
       </c>
     </row>
@@ -1019,25 +1029,25 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>100</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>9</v>
       </c>
     </row>
@@ -1045,25 +1055,25 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>95</v>
       </c>
     </row>
@@ -1071,25 +1081,25 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>66</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>2</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <v>9</v>
       </c>
     </row>
@@ -1097,25 +1107,25 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>4</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="8">
         <v>99</v>
       </c>
     </row>
@@ -1123,25 +1133,25 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>200</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="8">
         <v>5</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="8">
         <v>66</v>
       </c>
     </row>
@@ -1149,25 +1159,25 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>90</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>1</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="8">
         <v>80.599999999999994</v>
       </c>
     </row>
@@ -1175,25 +1185,25 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>88</v>
       </c>
     </row>
@@ -1201,25 +1211,25 @@
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="8">
         <v>64.400000000000006</v>
       </c>
     </row>
@@ -1227,25 +1237,25 @@
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>90</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>59</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="8">
         <v>60</v>
       </c>
     </row>
@@ -1253,25 +1263,25 @@
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="8">
         <v>1</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1279,25 +1289,25 @@
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="8">
         <v>2</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1305,25 +1315,25 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>80.599999999999994</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="8">
         <v>20</v>
       </c>
     </row>
@@ -1331,25 +1341,25 @@
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>100</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <v>10</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8">
         <v>88</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K16" s="9" t="s">
+      <c r="K16" s="8" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1357,19 +1367,19 @@
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <v>64.400000000000006</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="8">
         <v>70</v>
       </c>
     </row>
@@ -1377,13 +1387,13 @@
       <c r="G18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8">
         <v>60</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1391,13 +1401,13 @@
       <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="8" t="s">
         <v>58</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="8">
         <v>90</v>
       </c>
     </row>
@@ -1405,13 +1415,13 @@
       <c r="G20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H20" s="8" t="s">
         <v>59</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>80</v>
       </c>
     </row>
@@ -1419,13 +1429,13 @@
       <c r="G21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="9" t="s">
+      <c r="H21" s="8" t="s">
         <v>60</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="8">
         <v>66</v>
       </c>
     </row>
@@ -1433,13 +1443,13 @@
       <c r="G22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="9" t="s">
+      <c r="H22" s="8" t="s">
         <v>61</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="8">
         <v>60</v>
       </c>
     </row>
@@ -1447,13 +1457,13 @@
       <c r="G23" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>9</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="8">
         <v>50</v>
       </c>
     </row>
@@ -1461,13 +1471,13 @@
       <c r="G24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>99</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="8">
         <v>75</v>
       </c>
     </row>
@@ -1475,13 +1485,13 @@
       <c r="G25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <v>99</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <v>100</v>
       </c>
     </row>
@@ -1489,13 +1499,13 @@
       <c r="G26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <v>66</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <v>50</v>
       </c>
     </row>
@@ -1503,7 +1513,7 @@
       <c r="J27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="8">
         <v>80</v>
       </c>
     </row>
@@ -1511,33 +1521,33 @@
       <c r="J28" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="8">
         <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="J29" s="2"/>
-      <c r="K29" s="9"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11">
       <c r="J30" s="2"/>
-      <c r="K30" s="9"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11">
       <c r="J31" s="2"/>
-      <c r="K31" s="9"/>
+      <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11">
       <c r="J32" s="2"/>
-      <c r="K32" s="9"/>
+      <c r="K32" s="8"/>
     </row>
     <row r="33" spans="10:11">
       <c r="J33" s="2"/>
-      <c r="K33" s="9"/>
+      <c r="K33" s="8"/>
     </row>
     <row r="34" spans="10:11">
       <c r="J34" s="2"/>
-      <c r="K34" s="9"/>
+      <c r="K34" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1550,73 +1560,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="14" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="24" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="19"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="66" customHeight="1">
+    <row r="2" spans="1:9">
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1624,57 +1634,57 @@
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="18" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1682,28 +1692,28 @@
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="18" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1711,28 +1721,28 @@
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="18" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1740,45 +1750,45 @@
       <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="23"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="18" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1788,7 +1798,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{14A7592A-28A5-4DA8-BBFA-A088B6DA0243}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
@@ -1803,9 +1813,27 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{194D7DBB-6A47-4A01-B0E1-8E05DB433025}">
           <x14:formula1>
-            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+            <xm:f>commandinputdata!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C7</xm:sqref>
+          <xm:sqref>C6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{BD753466-73BF-4451-82EE-890AE8D0C768}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{2C238A52-CC3E-4BBB-845F-6B2DC73095B5}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{2BA85576-68CF-4034-A366-995061D9B116}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1817,131 +1845,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="14" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="24" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="19"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="66" customHeight="1">
+    <row r="2" spans="1:9">
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5">
+    <row r="3" spans="1:9" ht="29">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="18" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1949,28 +1977,28 @@
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="18" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1978,28 +2006,28 @@
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="18" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2007,45 +2035,45 @@
       <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="23"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="18" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2056,7 +2084,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{DE91018C-5078-4E02-9DE9-776D1975C9B1}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
@@ -2069,11 +2097,29 @@
           </x14:formula1>
           <xm:sqref>H3:H6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{E2DA3C6A-EFA3-42EE-B40E-65186E01436B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{33ED629C-6055-48FE-A7BD-AD3E2483F050}">
           <x14:formula1>
-            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+            <xm:f>commandinputdata!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C7</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{99006B66-5319-4228-9A35-20FD2B871684}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{9DE73CB4-AA26-4992-B3DB-24991CC26994}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{52B3BB8D-3345-4BB6-9F42-4D8F793B1B5F}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2085,131 +2131,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="14" style="19" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="24" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="19"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7265625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="66" customHeight="1">
+    <row r="2" spans="1:9">
       <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5">
+    <row r="3" spans="1:9" ht="29">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="43.5">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="18" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2217,28 +2263,28 @@
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="18" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2246,28 +2292,28 @@
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="18" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2275,45 +2321,45 @@
       <c r="A7" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="23"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="23" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="18" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2322,7 +2368,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{B0AA5AB9-597C-4DB1-A986-300FC9C6A1CB}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
@@ -2335,11 +2381,29 @@
           </x14:formula1>
           <xm:sqref>G2:G6 G8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{0FE8A086-DD56-4244-814A-05D86BAEBBF3}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{83BA2D7F-7AFE-464A-A8A6-0351BFE13AF0}">
           <x14:formula1>
-            <xm:f>commandinputdata!$C$2:$C$8</xm:f>
+            <xm:f>commandinputdata!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C7</xm:sqref>
+          <xm:sqref>C3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{D257DA1F-4547-4F03-B5ED-86D07266A34D}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$D$2:$D$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{59FBF960-3AF9-463F-BCCC-BA4A02F826D1}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{691E72CF-6304-4912-856A-BD3B2655C4F5}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2349,90 +2413,108 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DEF5F6-4C46-448A-BFCD-A11C30C672D9}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="18" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="18" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="23" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="C7" s="23" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="C8" s="23" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AUQA-64_DataValidation-updated as per review comments3
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C250763-E5DB-4AD4-90E2-40B0CCEB37D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D71ED5-5895-4AAF-9970-EE3A8E1D0782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
@@ -1560,7 +1560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1623,7 +1623,7 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
@@ -1650,7 +1650,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>106</v>
@@ -1679,7 +1679,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -1708,7 +1708,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -1737,7 +1737,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -1785,7 +1785,7 @@
         <v>124</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="18" t="s">
@@ -2131,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
override1 added to execution
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\fc\automation\AuQA\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38110BB3-EA81-4627-8CC6-159602F6DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DA3B97-93D3-43B7-8BCC-FC0BBB003C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="179">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -404,9 +404,6 @@
     <t>combinereport</t>
   </si>
   <si>
-    <t>GuardTest</t>
-  </si>
-  <si>
     <t>basichotGuard.xml/deadSensorGuard.xml/hotGuard.xml /guardOrderMIX.xml</t>
   </si>
   <si>
@@ -555,6 +552,33 @@
   </si>
   <si>
     <t>OFF</t>
+  </si>
+  <si>
+    <t>Override1</t>
+  </si>
+  <si>
+    <t>Override1_name</t>
+  </si>
+  <si>
+    <t>Override1_General-test</t>
+  </si>
+  <si>
+    <t>Overide1_Imputes-test</t>
+  </si>
+  <si>
+    <t>Overide1_RSP-test</t>
+  </si>
+  <si>
+    <t>override1.xml</t>
+  </si>
+  <si>
+    <t>basichotGuard.xml/deadSensorGuard.xml/hotGuard.xml /guardOrderMIX.xml/override1.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">override1.robot/staleStatePrevention.robot </t>
+  </si>
+  <si>
+    <t>Guard_Override_Test</t>
   </si>
 </sst>
 </file>
@@ -617,7 +641,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -640,11 +664,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -705,6 +740,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,23 +1023,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.77734375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="2.88671875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="2.88671875" style="14" customWidth="1"/>
-    <col min="10" max="10" width="23.21875" customWidth="1"/>
-    <col min="11" max="11" width="35.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.90625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.90625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" customWidth="1"/>
+    <col min="11" max="11" width="35.08984375" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -1032,7 +1068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8">
+    <row r="2" spans="1:11" ht="29">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1052,13 +1088,13 @@
         <v>1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" s="11">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.8">
+    <row r="3" spans="1:11" ht="29">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1078,13 +1114,13 @@
         <v>2</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K3" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="28.8">
+    <row r="4" spans="1:11" ht="43.5">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8">
+    <row r="5" spans="1:11" ht="29">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1136,7 +1172,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8">
+    <row r="6" spans="1:11" ht="29">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1162,7 +1198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.8">
+    <row r="7" spans="1:11" ht="29">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1188,7 +1224,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8">
+    <row r="8" spans="1:11" ht="29">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1214,7 +1250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="28.8">
+    <row r="9" spans="1:11" ht="29">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1276,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.8">
+    <row r="10" spans="1:11" ht="29">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1302,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="28.8">
+    <row r="11" spans="1:11" ht="29">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1292,7 +1328,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="28.8">
+    <row r="12" spans="1:11" ht="29">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1318,7 +1354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="57.6" customHeight="1">
+    <row r="13" spans="1:11" ht="57.65" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1344,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="28.8">
+    <row r="14" spans="1:11" ht="29">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1370,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="43.2">
+    <row r="15" spans="1:11" ht="43.5">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1396,7 +1432,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8">
+    <row r="16" spans="1:11" ht="29">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1442,7 +1478,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="28.8">
+    <row r="18" spans="1:11" ht="29">
       <c r="G18" s="2" t="s">
         <v>53</v>
       </c>
@@ -1456,7 +1492,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="28.8">
+    <row r="19" spans="1:11" ht="29">
       <c r="G19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1470,7 +1506,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8">
+    <row r="20" spans="1:11" ht="29">
       <c r="G20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1484,7 +1520,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.8">
+    <row r="21" spans="1:11" ht="29">
       <c r="G21" s="2" t="s">
         <v>23</v>
       </c>
@@ -1498,7 +1534,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="28.8">
+    <row r="22" spans="1:11" ht="29">
       <c r="G22" s="2" t="s">
         <v>24</v>
       </c>
@@ -1512,7 +1548,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="28.8">
+    <row r="23" spans="1:11" ht="29">
       <c r="G23" s="2" t="s">
         <v>54</v>
       </c>
@@ -1526,7 +1562,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="28.8">
+    <row r="24" spans="1:11" ht="29">
       <c r="G24" s="2" t="s">
         <v>55</v>
       </c>
@@ -1540,7 +1576,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="28.8">
+    <row r="25" spans="1:11" ht="29">
       <c r="G25" s="2" t="s">
         <v>56</v>
       </c>
@@ -1554,7 +1590,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="28.8">
+    <row r="26" spans="1:11" ht="29">
       <c r="G26" s="2" t="s">
         <v>57</v>
       </c>
@@ -1619,20 +1655,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D5FF25-CB93-4FF5-B7D2-AA3922F37E97}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.44140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.90625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
@@ -1656,7 +1692,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="4">
         <v>50</v>
@@ -1664,7 +1700,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="4">
         <v>100</v>
@@ -1720,7 +1756,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="4">
         <v>68</v>
@@ -1728,7 +1764,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12" s="4">
         <v>53</v>
@@ -1736,7 +1772,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B13" s="4">
         <v>72</v>
@@ -1744,7 +1780,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" s="4">
         <v>88</v>
@@ -1752,7 +1788,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>69</v>
@@ -1760,7 +1796,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" s="4">
         <v>77</v>
@@ -1768,15 +1804,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -1784,7 +1820,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -1792,7 +1828,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>72</v>
@@ -1800,7 +1836,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B21" s="4">
         <v>79</v>
@@ -1808,15 +1844,15 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>74</v>
@@ -1824,7 +1860,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B24" s="4">
         <v>81</v>
@@ -1832,10 +1868,10 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>169</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1845,24 +1881,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.77734375" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="16"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.81640625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1899,7 +1935,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -1910,22 +1946,22 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.2">
+    <row r="3" spans="1:9" ht="43.5">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -1937,7 +1973,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>106</v>
@@ -1946,12 +1982,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -1966,7 +2002,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -1975,12 +2011,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8">
+    <row r="5" spans="1:9" ht="29">
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -1995,7 +2031,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2004,12 +2040,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8">
+    <row r="6" spans="1:9" ht="29">
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2024,7 +2060,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2033,70 +2069,100 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6">
+    <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>135</v>
+        <v>126</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72.5">
+      <c r="A8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="B9" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F9" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="18" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{14A7592A-28A5-4DA8-BBFA-A088B6DA0243}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G8 G2:G6</xm:sqref>
+          <xm:sqref>G9 G2:G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{67438C2C-B12B-431F-81E3-DC6C78F3EFCA}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H6</xm:sqref>
+          <xm:sqref>H3:H7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{194D7DBB-6A47-4A01-B0E1-8E05DB433025}">
           <x14:formula1>
@@ -2122,6 +2188,12 @@
           </x14:formula1>
           <xm:sqref>C5</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{060A6CE4-8C5C-49B6-A2E8-601D6BB05769}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2130,24 +2202,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.5546875" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="16"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.54296875" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2184,7 +2256,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2195,22 +2267,22 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8">
+    <row r="3" spans="1:9" ht="29">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -2222,7 +2294,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>116</v>
@@ -2231,12 +2303,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -2251,7 +2323,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2260,12 +2332,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8">
+    <row r="5" spans="1:9" ht="29">
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -2280,7 +2352,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2289,12 +2361,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8">
+    <row r="6" spans="1:9" ht="29">
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2309,7 +2381,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2318,50 +2390,79 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6">
+    <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="58">
+      <c r="A8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="B9" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F9" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="18" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2371,18 +2472,18 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{DE91018C-5078-4E02-9DE9-776D1975C9B1}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G8 G2:G6</xm:sqref>
+          <xm:sqref>G9 G2:G7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{7B904523-E04A-4BBE-BEE8-FE5E9BFAB573}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H6</xm:sqref>
+          <xm:sqref>H3:H7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{33ED629C-6055-48FE-A7BD-AD3E2483F050}">
           <x14:formula1>
@@ -2408,6 +2509,12 @@
           </x14:formula1>
           <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{CE23025F-FF9C-4521-9EEB-D8CCE3E79E93}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2416,24 +2523,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="17" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.77734375" style="16" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="16"/>
+    <col min="1" max="1" width="15.08984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.81640625" style="16" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2470,7 +2577,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2481,22 +2588,22 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="28.8">
+    <row r="3" spans="1:9" ht="29">
       <c r="A3" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -2508,21 +2615,21 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8">
+    <row r="4" spans="1:9" ht="29">
       <c r="A4" s="21" t="s">
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -2537,7 +2644,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2546,12 +2653,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="28.8">
+    <row r="5" spans="1:9" ht="29">
       <c r="A5" s="21" t="s">
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -2566,7 +2673,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2575,12 +2682,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="28.8">
+    <row r="6" spans="1:9" ht="29">
       <c r="A6" s="21" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2595,7 +2702,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2604,50 +2711,79 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="57.6">
+    <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>137</v>
+        <v>126</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>170</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="58">
+      <c r="A8" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
+      <c r="B9" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F9" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18" t="s">
         <v>124</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="18" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2655,18 +2791,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{B0AA5AB9-597C-4DB1-A986-300FC9C6A1CB}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H6</xm:sqref>
+          <xm:sqref>H3:H7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{5BD409E9-D297-4950-9F42-71743EE745AC}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G6 G8</xm:sqref>
+          <xm:sqref>G2:G7 G9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{83BA2D7F-7AFE-464A-A8A6-0351BFE13AF0}">
           <x14:formula1>
@@ -2692,6 +2828,12 @@
           </x14:formula1>
           <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{438E4B38-BE5A-437C-9824-EF1D4461DD68}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2700,21 +2842,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DEF5F6-4C46-448A-BFCD-A11C30C672D9}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="12" t="s">
         <v>93</v>
       </c>
@@ -2722,30 +2866,33 @@
         <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>149</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>146</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>110</v>
@@ -2753,55 +2900,64 @@
       <c r="F2" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>102</v>
       </c>
       <c r="E3" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F4" s="18" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tursday and wednesday sheet updated
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DA3B97-93D3-43B7-8BCC-FC0BBB003C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1554B6-9462-4825-AF7B-E33DBED61413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="178">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -402,9 +402,6 @@
   </si>
   <si>
     <t>combinereport</t>
-  </si>
-  <si>
-    <t>basichotGuard.xml/deadSensorGuard.xml/hotGuard.xml /guardOrderMIX.xml</t>
   </si>
   <si>
     <t>moveReports</t>
@@ -1088,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K2" s="11">
         <v>50</v>
@@ -1114,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K3" s="11">
         <v>100</v>
@@ -1668,7 +1665,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
@@ -1692,7 +1689,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="4">
         <v>50</v>
@@ -1700,7 +1697,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="4">
         <v>100</v>
@@ -1756,7 +1753,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B11" s="4">
         <v>68</v>
@@ -1764,7 +1761,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="4">
         <v>53</v>
@@ -1772,7 +1769,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" s="4">
         <v>72</v>
@@ -1780,7 +1777,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B14" s="4">
         <v>88</v>
@@ -1788,7 +1785,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>69</v>
@@ -1796,7 +1793,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="4">
         <v>77</v>
@@ -1804,15 +1801,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -1820,7 +1817,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -1828,7 +1825,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>72</v>
@@ -1836,7 +1833,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" s="4">
         <v>79</v>
@@ -1844,15 +1841,15 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>74</v>
@@ -1860,7 +1857,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B24" s="4">
         <v>81</v>
@@ -1868,10 +1865,10 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1884,7 +1881,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1935,7 +1932,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -1946,7 +1943,7 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
@@ -1958,10 +1955,10 @@
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -1973,7 +1970,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>106</v>
@@ -1987,7 +1984,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -2002,7 +1999,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2016,7 +2013,7 @@
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -2031,7 +2028,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2045,7 +2042,7 @@
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2060,7 +2057,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2071,31 +2068,31 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72.5">
@@ -2103,19 +2100,19 @@
         <v>119</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2123,10 +2120,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -2134,14 +2131,14 @@
         <v>95</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2205,7 +2202,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2256,7 +2253,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2267,7 +2264,7 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
@@ -2279,10 +2276,10 @@
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -2294,7 +2291,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>116</v>
@@ -2308,7 +2305,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -2323,7 +2320,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2337,7 +2334,7 @@
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -2352,7 +2349,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2366,7 +2363,7 @@
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2381,7 +2378,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2392,51 +2389,51 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="58">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72.5">
       <c r="A8" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2444,10 +2441,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -2455,14 +2452,14 @@
         <v>95</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2525,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2577,7 +2574,7 @@
         <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
@@ -2588,7 +2585,7 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
@@ -2600,10 +2597,10 @@
         <v>89</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -2615,10 +2612,10 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I3" s="18" t="s">
         <v>99</v>
@@ -2629,7 +2626,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>102</v>
@@ -2644,7 +2641,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2658,7 +2655,7 @@
         <v>108</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>110</v>
@@ -2673,7 +2670,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2687,7 +2684,7 @@
         <v>109</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>111</v>
@@ -2702,7 +2699,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2713,51 +2710,51 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="58">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="72.5">
       <c r="A8" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2765,10 +2762,10 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -2776,14 +2773,14 @@
         <v>95</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2846,7 +2843,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2866,33 +2863,33 @@
         <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>110</v>
@@ -2901,63 +2898,63 @@
         <v>111</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>102</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tuesday suite updated with title for 146
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1554B6-9462-4825-AF7B-E33DBED61413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6C9E03-F246-4F78-83E3-109FA539DF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
@@ -443,9 +443,6 @@
     <t>RSP-test</t>
   </si>
   <si>
-    <t>Test performed on environment 37</t>
-  </si>
-  <si>
     <t>config37</t>
   </si>
   <si>
@@ -576,6 +573,9 @@
   </si>
   <si>
     <t>Guard_Override_Test</t>
+  </si>
+  <si>
+    <t>Test performed on environment 146</t>
   </si>
 </sst>
 </file>
@@ -1665,7 +1665,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="4">
         <v>68</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="4">
         <v>53</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="4">
         <v>72</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B14" s="4">
         <v>88</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>69</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="4">
         <v>77</v>
@@ -1801,15 +1801,15 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" s="4">
         <v>0</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>72</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21" s="4">
         <v>79</v>
@@ -1841,15 +1841,15 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>74</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B24" s="4">
         <v>81</v>
@@ -1865,10 +1865,10 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>167</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC20A92C-84F4-4904-85B3-A094CD26A426}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1943,7 +1943,7 @@
         <v>96</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="18" t="s">
@@ -1958,7 +1958,7 @@
         <v>125</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>94</v>
@@ -1970,7 +1970,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>106</v>
@@ -1999,7 +1999,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2028,7 +2028,7 @@
         <v>115</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="20" t="s">
         <v>116</v>
@@ -2057,7 +2057,7 @@
         <v>114</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="20" t="s">
         <v>116</v>
@@ -2068,31 +2068,31 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72.5">
@@ -2103,16 +2103,16 @@
         <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>177</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>133</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2134,7 +2134,7 @@
         <v>122</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="18" t="s">
@@ -2389,22 +2389,22 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>129</v>
@@ -2413,7 +2413,7 @@
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72.5">
@@ -2424,7 +2424,7 @@
         <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>130</v>
@@ -2433,7 +2433,7 @@
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2522,7 +2522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2612,7 +2612,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>132</v>
@@ -2641,7 +2641,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>106</v>
@@ -2710,31 +2710,31 @@
     </row>
     <row r="7" spans="1:9" ht="29">
       <c r="A7" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>125</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H7" s="20" t="s">
         <v>116</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="72.5">
@@ -2745,16 +2745,16 @@
         <v>121</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>104</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="19"/>
@@ -2863,24 +2863,24 @@
         <v>97</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="F1" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
         <v>116</v>
@@ -2889,7 +2889,7 @@
         <v>128</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>110</v>
@@ -2898,35 +2898,35 @@
         <v>111</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>102</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>132</v>
@@ -2935,16 +2935,16 @@
         <v>131</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2954,7 +2954,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rumode added to input sheet
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -5,19 +5,19 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\fc\automation\AuQA\Inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4185D9C-D08A-4DA9-A664-AE0047ADA194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B51A1E-9244-4A45-B176-E5831E836CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
     <sheet name="overrideTest" sheetId="7" r:id="rId2"/>
     <sheet name="tuesdaysuite" sheetId="8" r:id="rId3"/>
-    <sheet name="thursdaysuite" sheetId="2" r:id="rId4"/>
-    <sheet name="wednesdaysuite" sheetId="4" r:id="rId5"/>
+    <sheet name="wednesdaysuite" sheetId="4" r:id="rId4"/>
+    <sheet name="thursdaysuite" sheetId="2" r:id="rId5"/>
     <sheet name="commandinputdata" sheetId="6" r:id="rId6"/>
     <sheet name="testexecutioncommands" sheetId="9" r:id="rId7"/>
   </sheets>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="205">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -650,6 +650,18 @@
   <si>
     <t>sudo chmod 775 thursdayexecutesuite.sh
 sudo sh thursdayexecutesuite.sh</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>rumode</t>
   </si>
 </sst>
 </file>
@@ -750,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -826,6 +838,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1110,7 +1125,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1742,7 +1759,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1968,317 +1987,350 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF68788-F650-423E-ACA9-598F1A76ABAD}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.08984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.81640625" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="15"/>
+    <col min="2" max="2" width="9.26953125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.81640625" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="43.5">
+    <row r="3" spans="1:10" ht="43.5">
       <c r="A3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="I3" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="J3" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29">
+    <row r="4" spans="1:10" ht="29">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29">
+    <row r="5" spans="1:10" ht="29">
       <c r="A5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29">
+    <row r="6" spans="1:10" ht="29">
       <c r="A6" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29">
+    <row r="7" spans="1:10" ht="29">
       <c r="A7" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="I7" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="87">
+    <row r="8" spans="1:10" ht="87">
       <c r="A8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="17" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{2A443C34-7F60-4D1A-BEE9-2B2B19B10624}">
           <x14:formula1>
             <xm:f>commandinputdata!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{A3AF2C92-0953-4D86-9DBA-F4C811F9BD2A}">
           <x14:formula1>
             <xm:f>commandinputdata!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{7F8D7859-404D-4475-BC34-50E3A878DCA3}">
           <x14:formula1>
             <xm:f>commandinputdata!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{115AFEBA-9626-4203-AD1B-AAF35A5B2992}">
           <x14:formula1>
             <xm:f>commandinputdata!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{A8E9437C-6530-4719-A1E0-546D00E7EB7B}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G9 G2:G7</xm:sqref>
+          <xm:sqref>H9 H2:H7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{0EB62EF6-1A00-44DA-A84D-00E569387EB6}">
           <x14:formula1>
             <xm:f>commandinputdata!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>D7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{98B96F75-8CE1-40CB-8870-67B1472C5745}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H7</xm:sqref>
+          <xm:sqref>I3:I7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7EEF3ED2-772E-4D4C-844E-E25E0DF81A1E}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2287,318 +2339,351 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.08984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.54296875" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="15"/>
+    <col min="2" max="2" width="9.26953125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.81640625" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29">
+    <row r="3" spans="1:10" ht="29">
       <c r="A3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>129</v>
-      </c>
       <c r="H3" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="I3" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29">
+    <row r="4" spans="1:10" ht="29">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>129</v>
-      </c>
       <c r="H4" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29">
+    <row r="5" spans="1:10" ht="29">
       <c r="A5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29">
+    <row r="6" spans="1:10" ht="29">
       <c r="A6" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29">
+    <row r="7" spans="1:10" ht="29">
       <c r="A7" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>129</v>
-      </c>
       <c r="H7" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="72.5">
+    <row r="8" spans="1:10" ht="87">
       <c r="A8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>130</v>
-      </c>
       <c r="E8" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="17" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{DE91018C-5078-4E02-9DE9-776D1975C9B1}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{B0AA5AB9-597C-4DB1-A986-300FC9C6A1CB}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I3:I7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{5BD409E9-D297-4950-9F42-71743EE745AC}">
           <x14:formula1>
             <xm:f>commandinputdata!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>G9 G2:G7</xm:sqref>
+          <xm:sqref>H2:H7 H9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{7B904523-E04A-4BBE-BEE8-FE5E9BFAB573}">
-          <x14:formula1>
-            <xm:f>commandinputdata!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H3:H7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{33ED629C-6055-48FE-A7BD-AD3E2483F050}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{83BA2D7F-7AFE-464A-A8A6-0351BFE13AF0}">
           <x14:formula1>
             <xm:f>commandinputdata!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{99006B66-5319-4228-9A35-20FD2B871684}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{D257DA1F-4547-4F03-B5ED-86D07266A34D}">
           <x14:formula1>
             <xm:f>commandinputdata!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{9DE73CB4-AA26-4992-B3DB-24991CC26994}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{59FBF960-3AF9-463F-BCCC-BA4A02F826D1}">
           <x14:formula1>
             <xm:f>commandinputdata!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{52B3BB8D-3345-4BB6-9F42-4D8F793B1B5F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{691E72CF-6304-4912-856A-BD3B2655C4F5}">
           <x14:formula1>
             <xm:f>commandinputdata!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{CE23025F-FF9C-4521-9EEB-D8CCE3E79E93}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{438E4B38-BE5A-437C-9824-EF1D4461DD68}">
           <x14:formula1>
             <xm:f>commandinputdata!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FE359760-DBB1-446F-9D96-28A7C4B1C13D}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2607,318 +2692,353 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42037A05-F46D-4E48-89CA-F63CAC18AB6B}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96345453-F080-4B9E-8403-62D273ADBBA7}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="15.08984375" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.81640625" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="15"/>
+    <col min="2" max="2" width="9.26953125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.81640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.08984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.54296875" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="8.81640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="23" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="18"/>
+      <c r="J2" s="17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29">
+    <row r="3" spans="1:10" ht="29">
       <c r="A3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="H3" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29">
+    <row r="4" spans="1:10" ht="29">
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>135</v>
-      </c>
       <c r="H4" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="J4" s="17" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29">
+    <row r="5" spans="1:10" ht="29">
       <c r="A5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="H5" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="I5" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="29">
+    <row r="6" spans="1:10" ht="29">
       <c r="A6" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="G6" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="H6" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="I6" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="J6" s="17" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29">
+    <row r="7" spans="1:10" ht="29">
       <c r="A7" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="D7" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="F7" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="G7" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="19" t="s">
-        <v>135</v>
-      </c>
       <c r="H7" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="87">
+    <row r="8" spans="1:10" ht="72.5">
       <c r="A8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>134</v>
-      </c>
       <c r="E8" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="18"/>
+      <c r="J9" s="17" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{B0AA5AB9-597C-4DB1-A986-300FC9C6A1CB}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{DE91018C-5078-4E02-9DE9-776D1975C9B1}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>H9 H2:H7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Group" xr:uid="{7B904523-E04A-4BBE-BEE8-FE5E9BFAB573}">
           <x14:formula1>
             <xm:f>commandinputdata!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H3:H7</xm:sqref>
+          <xm:sqref>I3:I7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Environment" xr:uid="{5BD409E9-D297-4950-9F42-71743EE745AC}">
-          <x14:formula1>
-            <xm:f>commandinputdata!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G7 G9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{83BA2D7F-7AFE-464A-A8A6-0351BFE13AF0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{33ED629C-6055-48FE-A7BD-AD3E2483F050}">
           <x14:formula1>
             <xm:f>commandinputdata!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C3</xm:sqref>
+          <xm:sqref>D3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{D257DA1F-4547-4F03-B5ED-86D07266A34D}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{99006B66-5319-4228-9A35-20FD2B871684}">
           <x14:formula1>
             <xm:f>commandinputdata!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
+          <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{59FBF960-3AF9-463F-BCCC-BA4A02F826D1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{9DE73CB4-AA26-4992-B3DB-24991CC26994}">
           <x14:formula1>
             <xm:f>commandinputdata!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C5</xm:sqref>
+          <xm:sqref>D5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{691E72CF-6304-4912-856A-BD3B2655C4F5}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{52B3BB8D-3345-4BB6-9F42-4D8F793B1B5F}">
           <x14:formula1>
             <xm:f>commandinputdata!$F$2:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C6</xm:sqref>
+          <xm:sqref>D6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{438E4B38-BE5A-437C-9824-EF1D4461DD68}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select a value from drop down list" prompt="Select Name" xr:uid="{CE23025F-FF9C-4521-9EEB-D8CCE3E79E93}">
           <x14:formula1>
             <xm:f>commandinputdata!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>D7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5126730B-CD13-4170-97B7-B0ACEDBDE549}">
+          <x14:formula1>
+            <xm:f>commandinputdata!$H$2:$H$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2929,11 +3049,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DEF5F6-4C46-448A-BFCD-A11C30C672D9}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2945,7 +3065,7 @@
     <col min="8" max="8" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="12" t="s">
         <v>93</v>
       </c>
@@ -2967,8 +3087,11 @@
       <c r="G1" s="22" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>133</v>
       </c>
@@ -2990,8 +3113,11 @@
       <c r="G2" s="17" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>137</v>
       </c>
@@ -3013,8 +3139,11 @@
       <c r="G3" s="17" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>135</v>
       </c>
@@ -3037,18 +3166,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3059,8 +3187,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
updated all yes to thursdaysuite
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B51A1E-9244-4A45-B176-E5831E836CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3BF7FA-DFC8-43CC-8580-51771EEC355D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
@@ -1125,7 +1125,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1989,8 +1989,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2279,6 +2279,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -2344,7 +2345,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2633,6 +2634,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2696,8 +2698,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2751,7 +2753,7 @@
       <c r="A2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="29" t="s">
         <v>202</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -2777,8 +2779,8 @@
       <c r="A3" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="20" t="s">
-        <v>203</v>
+      <c r="B3" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>125</v>
@@ -2809,8 +2811,8 @@
       <c r="A4" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>203</v>
+      <c r="B4" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>125</v>
@@ -2841,8 +2843,8 @@
       <c r="A5" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>203</v>
+      <c r="B5" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>125</v>
@@ -2873,8 +2875,8 @@
       <c r="A6" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>203</v>
+      <c r="B6" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>125</v>
@@ -2905,8 +2907,8 @@
       <c r="A7" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>203</v>
+      <c r="B7" s="29" t="s">
+        <v>202</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>125</v>
@@ -2937,7 +2939,7 @@
       <c r="A8" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="29" t="s">
         <v>202</v>
       </c>
       <c r="C8" s="17" t="s">
@@ -2963,7 +2965,7 @@
       <c r="A9" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="29" t="s">
         <v>202</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -2986,6 +2988,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3053,7 +3056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3177,6 +3180,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3187,8 +3191,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Tc commented for testrun
</commit_message>
<xml_diff>
--- a/Inputs/testInputs.xlsx
+++ b/Inputs/testInputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\home\fc\automation\AuQA\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5C781-C772-47ED-B748-962B013970E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0021E239-E804-4466-994C-CA3784DD6286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="guardTest" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="342">
   <si>
     <t>basicHotAbsoluteGuardInputs</t>
   </si>
@@ -861,9 +861,6 @@
 Override all equipment for group General-test to the configured maximum cooling level?</t>
   </si>
   <si>
-    <t>sudo robot --name 'Popup' --reporttitle "Popups" --outputdir Reports --output uiPopup.xml --variable environment:config37 -v groupname:General-test -T /home/fc/automation/AuQA/Testcases/UITests/uiPopupTest.robot</t>
-  </si>
-  <si>
     <t>Alarm subject 00-17-0D-00-00-1A-C8-A0 is not bound to any assets.</t>
   </si>
   <si>
@@ -945,9 +942,6 @@
     <t>sudo pabot --pabotlib --processes 2 --name 'Override_MinOnNoBindings-test'  --reporttitle "MinOnNoBindings"  --outputdir Reports --output minOnNoBindings.xml --variable environment:config146 -v groupname:NoBindings -T /home/fc/automation/AuQA/Testcases/OverrideTests/minOnNoBindingsTest.robot /home/fc/automation/AuQA/Testcases/staleStatePrevention.robot</t>
   </si>
   <si>
-    <t>sudo robot --name 'Override_MinOnGeneral-test'  --reporttitle "MinOnGeneral"  --outputdir Reports --output minOnGeneral.xml --variable environment:config146 -v groupname:General-test /home/fc/automation/AuQA/Testcases/OverrideTests/minOnGeneralTest.robot</t>
-  </si>
-  <si>
     <t>sudo rebot --removekeywords passed --name 'Guard_Override_Test' --reporttitle "Test performed on environment 37" --outputdir Reports --output output.xml /home/fc/automation/AuQA/Reports/basichotGuard.xml /home/fc/automation/AuQA/Reports/deadSensorGuard.xml /home/fc/automation/AuQA/Reports/hotGuard.xml /home/fc/automation/AuQA/Reports/guardOrderMIX.xml /home/fc/automation/AuQA/Reports/vxOverrideUIvalues.xml /home/fc/automation/AuQA/Testcases/UITests/uiPopup.xml /home/fc/automation/AuQA/Testcases/OverrideTests/minOnNoBindingsTest.robot /home/fc/automation/AuQA/Testcases/OverrideTests/minOnGeneralTest.robot</t>
   </si>
   <si>
@@ -997,6 +991,90 @@
   </si>
   <si>
     <t>ahu_property_onpwrlvl_default</t>
+  </si>
+  <si>
+    <t>rack_intial_tempF</t>
+  </si>
+  <si>
+    <t>power_monitor_on_pwr_kW</t>
+  </si>
+  <si>
+    <t>rack_cold_tempF</t>
+  </si>
+  <si>
+    <t>alarm_off</t>
+  </si>
+  <si>
+    <t>alarm_on</t>
+  </si>
+  <si>
+    <t>group_cold_alarm</t>
+  </si>
+  <si>
+    <t>GroupCold</t>
+  </si>
+  <si>
+    <t>groupColdAlarmTestInputs</t>
+  </si>
+  <si>
+    <t>groupDeadSensorTestInputs</t>
+  </si>
+  <si>
+    <t>group_dead_sensor_alarm</t>
+  </si>
+  <si>
+    <t>GroupDeadSensor</t>
+  </si>
+  <si>
+    <t>num_minutes_past_default</t>
+  </si>
+  <si>
+    <t>sudo pabot --pabotlib --processes 1 --name 'Popup' --reporttitle "Popups" --outputdir Reports --output uiPopup.xml --variable environment:config37 -v groupname:General-test -T /home/fc/automation/AuQA/Testcases/UITests/uiPopupTest.robot</t>
+  </si>
+  <si>
+    <t>sudo pabot --pabotlib --processes 1 --name 'Override_MinOnGeneral-test'  --reporttitle "MinOnGeneral"  --outputdir Reports --output minOnGeneral.xml --variable environment:config146 -v groupname:General-test /home/fc/automation/AuQA/Testcases/OverrideTests/minOnGeneralTest.robot</t>
+  </si>
+  <si>
+    <t>validation_error_popup_title</t>
+  </si>
+  <si>
+    <t>Validation Error</t>
+  </si>
+  <si>
+    <t>sfcmin_popup_message</t>
+  </si>
+  <si>
+    <t>SYSTEM.SFCMin: The value must not be blank.</t>
+  </si>
+  <si>
+    <t>save_popup_title</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>save_popup_message</t>
+  </si>
+  <si>
+    <t>Nothing to save.</t>
+  </si>
+  <si>
+    <t>turn_off_limit_24_hr_popup_message</t>
+  </si>
+  <si>
+    <t>DASHM.TurnOffLimit24H: The unsigned integer is below the minimum of 0</t>
+  </si>
+  <si>
+    <t>unsaved_changes_popup_title</t>
+  </si>
+  <si>
+    <t>Unsaved Changes</t>
+  </si>
+  <si>
+    <t>unsaved_changes_popup_message</t>
+  </si>
+  <si>
+    <t>Discard changes before closing this window?</t>
   </si>
   <si>
     <t>combinexml</t>
@@ -1100,7 +1178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1180,6 +1258,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1465,7 +1550,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2099,7 +2184,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2129,7 +2214,7 @@
         <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>17</v>
@@ -2228,13 +2313,13 @@
         <v>227</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G6" s="19" t="s">
         <v>227</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2394,7 +2479,7 @@
         <v>235</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2574,7 +2659,7 @@
         <v>69</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2594,7 +2679,7 @@
         <v>70</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2614,7 +2699,7 @@
         <v>71</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2628,7 +2713,7 @@
         <v>72</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2638,7 +2723,7 @@
         <v>73</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2648,7 +2733,7 @@
         <v>74</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2656,7 +2741,7 @@
         <v>75</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2664,7 +2749,7 @@
         <v>76</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2675,144 +2760,313 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1213F30C-9986-413F-9139-B40DA43E91F9}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="38.453125" customWidth="1"/>
     <col min="2" max="2" width="29.90625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="2.90625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="38.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="2.90625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="38.453125" customWidth="1"/>
+    <col min="8" max="8" width="16" style="7" customWidth="1"/>
+    <col min="9" max="9" width="2.90625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="D1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="H3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="19" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B4" s="4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="4">
         <v>80.599999999999994</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="4">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="4">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="4">
         <v>64.400000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="4">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="4">
+        <v>64.400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="19" t="s">
         <v>229</v>
       </c>
       <c r="B7" s="4">
         <v>80.599999999999994</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="D7" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="4">
+        <v>86</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="H7" s="4">
+        <v>80.599999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="19" t="s">
         <v>150</v>
       </c>
       <c r="B8" s="4">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="D8" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="4">
+        <v>76</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="19" t="s">
         <v>151</v>
       </c>
       <c r="B9" s="4">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D9" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="4">
+        <v>10</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="H9" s="4">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B10" s="4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="D10" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E10" s="4">
+        <v>34</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="H10" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="D11" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>304</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B13" s="4">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="H14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="19" t="s">
+    <row r="16" spans="1:8" ht="43.5">
+      <c r="A16" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="43.5">
-      <c r="A16" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2831,8 +3085,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -2886,7 +3140,7 @@
       <c r="A2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3076,7 +3330,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>219</v>
@@ -3102,7 +3356,7 @@
     </row>
     <row r="9" spans="1:10" ht="29">
       <c r="A9" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>200</v>
@@ -3111,48 +3365,48 @@
         <v>125</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>138</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29">
       <c r="A10" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>200</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>138</v>
@@ -3161,14 +3415,14 @@
         <v>116</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="29">
       <c r="A11" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -3184,7 +3438,7 @@
         <v>104</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
@@ -3194,7 +3448,7 @@
       <c r="A12" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -3269,7 +3523,7 @@
           <x14:formula1>
             <xm:f>commandinputdata!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B12</xm:sqref>
+          <xm:sqref>B3:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3282,8 +3536,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3337,7 +3591,7 @@
       <c r="A2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3524,10 +3778,10 @@
         <v>223</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>219</v>
@@ -3553,7 +3807,7 @@
     </row>
     <row r="9" spans="1:10" ht="29">
       <c r="A9" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>200</v>
@@ -3562,48 +3816,48 @@
         <v>125</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>138</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29">
       <c r="A10" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>200</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>138</v>
@@ -3612,14 +3866,14 @@
         <v>116</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.5">
       <c r="A11" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -3635,7 +3889,7 @@
         <v>104</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>315</v>
+        <v>341</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
@@ -3645,7 +3899,7 @@
       <c r="A12" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -3720,7 +3974,7 @@
           <x14:formula1>
             <xm:f>commandinputdata!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B12</xm:sqref>
+          <xm:sqref>B3:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3733,8 +3987,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3788,7 +4042,7 @@
       <c r="A2" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -3978,7 +4232,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>219</v>
@@ -4004,7 +4258,7 @@
     </row>
     <row r="9" spans="1:10" ht="29">
       <c r="A9" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>200</v>
@@ -4013,48 +4267,48 @@
         <v>125</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>138</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29">
       <c r="A10" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>200</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>104</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>138</v>
@@ -4063,14 +4317,14 @@
         <v>116</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="29">
       <c r="A11" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C11" s="15" t="s">
@@ -4085,8 +4339,8 @@
       <c r="F11" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>315</v>
+      <c r="G11" s="15" t="s">
+        <v>341</v>
       </c>
       <c r="H11" s="15"/>
       <c r="I11" s="16"/>
@@ -4096,7 +4350,7 @@
       <c r="A12" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="34" t="s">
         <v>200</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -4172,7 +4426,7 @@
           <x14:formula1>
             <xm:f>commandinputdata!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B12</xm:sqref>
+          <xm:sqref>B3:B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4187,7 +4441,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4305,7 +4559,7 @@
         <v>129</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -4325,7 +4579,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
@@ -4395,23 +4651,23 @@
         <v>223</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>269</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="58">
       <c r="A9" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.5">
+      <c r="A10" s="30" t="s">
         <v>293</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="29">
-      <c r="A10" s="30" t="s">
-        <v>294</v>
-      </c>
       <c r="B10" s="22" t="s">
-        <v>297</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="87">
@@ -4419,7 +4675,7 @@
         <v>182</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29">
@@ -4483,9 +4739,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700C9353-2A30-431F-BC2E-391121D039E2}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -4623,18 +4881,74 @@
     </row>
     <row r="17" spans="1:2" ht="29">
       <c r="A17" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="29">
+      <c r="A23" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>